<commit_message>
Minor textual updates during review
</commit_message>
<xml_diff>
--- a/01_windstorm/LUISA_damage_info_curves.xlsx
+++ b/01_windstorm/LUISA_damage_info_curves.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26529"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27628"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://deltares-my.sharepoint.com/personal/ted_buskop_deltares_nl/Documents/Documents/GitHub/STORMS/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aleksand\git_projects\CLIMAAX\STORMS\01_windstorm\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="3" documentId="11_E3781DF3B754BDB79EE7DCCFC647EB92B7130EFD" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{792C5A67-9E70-4BDB-9B0A-12E7F1A667E7}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A5A23C3-258C-4A8C-A7B3-1C7C8B2AD45C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-165" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -290,7 +290,7 @@
     <numFmt numFmtId="165" formatCode="#,##0%"/>
     <numFmt numFmtId="166" formatCode="#,##0.00%"/>
   </numFmts>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -322,8 +322,13 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -343,6 +348,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -380,7 +391,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="1" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -435,6 +446,9 @@
     </xf>
     <xf numFmtId="2" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="2" fontId="5" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -743,9 +757,9 @@
   </sheetPr>
   <dimension ref="A1:AI47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="O17" sqref="O17"/>
+      <selection pane="bottomLeft" activeCell="I8" sqref="I8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -897,7 +911,7 @@
       <c r="B2" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="C2" s="17">
+      <c r="C2" s="19">
         <v>32169</v>
       </c>
       <c r="D2" s="17">
@@ -1014,6 +1028,7 @@
         <v>36</v>
       </c>
       <c r="C3" s="17">
+        <f>C$2</f>
         <v>32169</v>
       </c>
       <c r="D3" s="17">
@@ -1130,6 +1145,7 @@
         <v>37</v>
       </c>
       <c r="C4" s="17">
+        <f t="shared" ref="C4:C47" si="9">C$2</f>
         <v>32169</v>
       </c>
       <c r="D4" s="17">
@@ -1246,6 +1262,7 @@
         <v>38</v>
       </c>
       <c r="C5" s="17">
+        <f t="shared" si="9"/>
         <v>32169</v>
       </c>
       <c r="D5" s="17">
@@ -1362,6 +1379,7 @@
         <v>39</v>
       </c>
       <c r="C6" s="17">
+        <f t="shared" si="9"/>
         <v>32169</v>
       </c>
       <c r="D6" s="17">
@@ -1478,6 +1496,7 @@
         <v>40</v>
       </c>
       <c r="C7" s="17">
+        <f t="shared" si="9"/>
         <v>32169</v>
       </c>
       <c r="D7" s="17">
@@ -1594,6 +1613,7 @@
         <v>41</v>
       </c>
       <c r="C8" s="17">
+        <f t="shared" si="9"/>
         <v>32169</v>
       </c>
       <c r="D8" s="17">
@@ -1710,6 +1730,7 @@
         <v>42</v>
       </c>
       <c r="C9" s="17">
+        <f t="shared" si="9"/>
         <v>32169</v>
       </c>
       <c r="D9" s="17">
@@ -1826,6 +1847,7 @@
         <v>43</v>
       </c>
       <c r="C10" s="17">
+        <f t="shared" si="9"/>
         <v>32169</v>
       </c>
       <c r="D10" s="17">
@@ -1942,6 +1964,7 @@
         <v>44</v>
       </c>
       <c r="C11" s="17">
+        <f t="shared" si="9"/>
         <v>32169</v>
       </c>
       <c r="D11" s="17">
@@ -2058,6 +2081,7 @@
         <v>45</v>
       </c>
       <c r="C12" s="17">
+        <f t="shared" si="9"/>
         <v>32169</v>
       </c>
       <c r="D12" s="17">
@@ -2174,6 +2198,7 @@
         <v>46</v>
       </c>
       <c r="C13" s="17">
+        <f t="shared" si="9"/>
         <v>32169</v>
       </c>
       <c r="D13" s="17">
@@ -2290,6 +2315,7 @@
         <v>47</v>
       </c>
       <c r="C14" s="17">
+        <f t="shared" si="9"/>
         <v>32169</v>
       </c>
       <c r="D14" s="17">
@@ -2406,6 +2432,7 @@
         <v>48</v>
       </c>
       <c r="C15" s="17">
+        <f t="shared" si="9"/>
         <v>32169</v>
       </c>
       <c r="D15" s="17">
@@ -2522,6 +2549,7 @@
         <v>49</v>
       </c>
       <c r="C16" s="17">
+        <f t="shared" si="9"/>
         <v>32169</v>
       </c>
       <c r="D16" s="17">
@@ -2638,6 +2666,7 @@
         <v>50</v>
       </c>
       <c r="C17" s="17">
+        <f t="shared" si="9"/>
         <v>32169</v>
       </c>
       <c r="D17" s="17">
@@ -2754,6 +2783,7 @@
         <v>51</v>
       </c>
       <c r="C18" s="17">
+        <f t="shared" si="9"/>
         <v>32169</v>
       </c>
       <c r="D18" s="17">
@@ -2870,6 +2900,7 @@
         <v>52</v>
       </c>
       <c r="C19" s="17">
+        <f t="shared" si="9"/>
         <v>32169</v>
       </c>
       <c r="D19" s="17">
@@ -2944,7 +2975,7 @@
         <v>16.529354868081764</v>
       </c>
       <c r="Y19" s="17">
-        <f t="shared" ref="Y19:Y29" si="9">0.1015744</f>
+        <f t="shared" ref="Y19:Y29" si="10">0.1015744</f>
         <v>0.1015744</v>
       </c>
       <c r="Z19" s="17">
@@ -2987,6 +3018,7 @@
         <v>53</v>
       </c>
       <c r="C20" s="17">
+        <f t="shared" si="9"/>
         <v>32169</v>
       </c>
       <c r="D20" s="17">
@@ -3061,7 +3093,7 @@
         <v>16.529354868081764</v>
       </c>
       <c r="Y20" s="17">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>0.1015744</v>
       </c>
       <c r="Z20" s="17">
@@ -3104,6 +3136,7 @@
         <v>54</v>
       </c>
       <c r="C21" s="17">
+        <f t="shared" si="9"/>
         <v>32169</v>
       </c>
       <c r="D21" s="17">
@@ -3178,7 +3211,7 @@
         <v>16.529354868081764</v>
       </c>
       <c r="Y21" s="17">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>0.1015744</v>
       </c>
       <c r="Z21" s="17">
@@ -3221,6 +3254,7 @@
         <v>55</v>
       </c>
       <c r="C22" s="17">
+        <f t="shared" si="9"/>
         <v>32169</v>
       </c>
       <c r="D22" s="17">
@@ -3295,7 +3329,7 @@
         <v>16.529354868081764</v>
       </c>
       <c r="Y22" s="17">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>0.1015744</v>
       </c>
       <c r="Z22" s="17">
@@ -3338,6 +3372,7 @@
         <v>56</v>
       </c>
       <c r="C23" s="17">
+        <f t="shared" si="9"/>
         <v>32169</v>
       </c>
       <c r="D23" s="17">
@@ -3412,7 +3447,7 @@
         <v>16.529354868081764</v>
       </c>
       <c r="Y23" s="17">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>0.1015744</v>
       </c>
       <c r="Z23" s="17">
@@ -3455,6 +3490,7 @@
         <v>57</v>
       </c>
       <c r="C24" s="17">
+        <f t="shared" si="9"/>
         <v>32169</v>
       </c>
       <c r="D24" s="17">
@@ -3529,7 +3565,7 @@
         <v>16.529354868081764</v>
       </c>
       <c r="Y24" s="17">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>0.1015744</v>
       </c>
       <c r="Z24" s="17">
@@ -3572,6 +3608,7 @@
         <v>58</v>
       </c>
       <c r="C25" s="17">
+        <f t="shared" si="9"/>
         <v>32169</v>
       </c>
       <c r="D25" s="17">
@@ -3646,7 +3683,7 @@
         <v>16.529354868081764</v>
       </c>
       <c r="Y25" s="17">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>0.1015744</v>
       </c>
       <c r="Z25" s="17">
@@ -3689,6 +3726,7 @@
         <v>59</v>
       </c>
       <c r="C26" s="17">
+        <f t="shared" si="9"/>
         <v>32169</v>
       </c>
       <c r="D26" s="17">
@@ -3763,7 +3801,7 @@
         <v>16.529354868081764</v>
       </c>
       <c r="Y26" s="17">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>0.1015744</v>
       </c>
       <c r="Z26" s="17">
@@ -3806,6 +3844,7 @@
         <v>60</v>
       </c>
       <c r="C27" s="17">
+        <f t="shared" si="9"/>
         <v>32169</v>
       </c>
       <c r="D27" s="17">
@@ -3880,7 +3919,7 @@
         <v>16.529354868081764</v>
       </c>
       <c r="Y27" s="17">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>0.1015744</v>
       </c>
       <c r="Z27" s="17">
@@ -3923,6 +3962,7 @@
         <v>61</v>
       </c>
       <c r="C28" s="17">
+        <f t="shared" si="9"/>
         <v>32169</v>
       </c>
       <c r="D28" s="17">
@@ -3997,7 +4037,7 @@
         <v>16.529354868081764</v>
       </c>
       <c r="Y28" s="17">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>0.1015744</v>
       </c>
       <c r="Z28" s="17">
@@ -4040,6 +4080,7 @@
         <v>62</v>
       </c>
       <c r="C29" s="17">
+        <f t="shared" si="9"/>
         <v>32169</v>
       </c>
       <c r="D29" s="17">
@@ -4114,7 +4155,7 @@
         <v>16.529354868081764</v>
       </c>
       <c r="Y29" s="17">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>0.1015744</v>
       </c>
       <c r="Z29" s="17">
@@ -4157,6 +4198,7 @@
         <v>63</v>
       </c>
       <c r="C30" s="17">
+        <f t="shared" si="9"/>
         <v>32169</v>
       </c>
       <c r="D30" s="17">
@@ -4273,6 +4315,7 @@
         <v>64</v>
       </c>
       <c r="C31" s="17">
+        <f t="shared" si="9"/>
         <v>32169</v>
       </c>
       <c r="D31" s="17">
@@ -4389,6 +4432,7 @@
         <v>65</v>
       </c>
       <c r="C32" s="17">
+        <f t="shared" si="9"/>
         <v>32169</v>
       </c>
       <c r="D32" s="17">
@@ -4505,6 +4549,7 @@
         <v>66</v>
       </c>
       <c r="C33" s="17">
+        <f t="shared" si="9"/>
         <v>32169</v>
       </c>
       <c r="D33" s="17">
@@ -4621,6 +4666,7 @@
         <v>67</v>
       </c>
       <c r="C34" s="17">
+        <f t="shared" si="9"/>
         <v>32169</v>
       </c>
       <c r="D34" s="17">
@@ -4737,6 +4783,7 @@
         <v>68</v>
       </c>
       <c r="C35" s="17">
+        <f t="shared" si="9"/>
         <v>32169</v>
       </c>
       <c r="D35" s="17">
@@ -4853,6 +4900,7 @@
         <v>69</v>
       </c>
       <c r="C36" s="17">
+        <f t="shared" si="9"/>
         <v>32169</v>
       </c>
       <c r="D36" s="17">
@@ -4969,6 +5017,7 @@
         <v>70</v>
       </c>
       <c r="C37" s="17">
+        <f t="shared" si="9"/>
         <v>32169</v>
       </c>
       <c r="D37" s="17">
@@ -5085,6 +5134,7 @@
         <v>71</v>
       </c>
       <c r="C38" s="17">
+        <f t="shared" si="9"/>
         <v>32169</v>
       </c>
       <c r="D38" s="17">
@@ -5201,6 +5251,7 @@
         <v>72</v>
       </c>
       <c r="C39" s="17">
+        <f t="shared" si="9"/>
         <v>32169</v>
       </c>
       <c r="D39" s="17">
@@ -5317,6 +5368,7 @@
         <v>73</v>
       </c>
       <c r="C40" s="17">
+        <f t="shared" si="9"/>
         <v>32169</v>
       </c>
       <c r="D40" s="17">
@@ -5433,6 +5485,7 @@
         <v>74</v>
       </c>
       <c r="C41" s="17">
+        <f t="shared" si="9"/>
         <v>32169</v>
       </c>
       <c r="D41" s="17">
@@ -5549,6 +5602,7 @@
         <v>75</v>
       </c>
       <c r="C42" s="17">
+        <f t="shared" si="9"/>
         <v>32169</v>
       </c>
       <c r="D42" s="17">
@@ -5665,6 +5719,7 @@
         <v>76</v>
       </c>
       <c r="C43" s="17">
+        <f t="shared" si="9"/>
         <v>32169</v>
       </c>
       <c r="D43" s="17">
@@ -5781,6 +5836,7 @@
         <v>77</v>
       </c>
       <c r="C44" s="17">
+        <f t="shared" si="9"/>
         <v>32169</v>
       </c>
       <c r="D44" s="17">
@@ -5897,6 +5953,7 @@
         <v>78</v>
       </c>
       <c r="C45" s="17">
+        <f t="shared" si="9"/>
         <v>32169</v>
       </c>
       <c r="D45" s="17">
@@ -6013,6 +6070,7 @@
         <v>79</v>
       </c>
       <c r="C46" s="17">
+        <f t="shared" si="9"/>
         <v>32169</v>
       </c>
       <c r="D46" s="17">
@@ -6129,6 +6187,7 @@
         <v>80</v>
       </c>
       <c r="C47" s="17">
+        <f t="shared" si="9"/>
         <v>32169</v>
       </c>
       <c r="D47" s="17">

</xml_diff>

<commit_message>
fix: adjust build up area density in farm areas according to spanish situation.
</commit_message>
<xml_diff>
--- a/01_windstorm/LUISA_damage_info_curves.xlsx
+++ b/01_windstorm/LUISA_damage_info_curves.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10511"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="28925"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ecm5975/CLIMAAX/STORMS/01_windstorm/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://deltares-my.sharepoint.com/personal/ted_buskop_deltares_nl/Documents/Documents/GitHub/STORMS/01_windstorm/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98380BDD-C188-254D-82D1-BBEECDE7A39E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="12" documentId="13_ncr:1_{98380BDD-C188-254D-82D1-BBEECDE7A39E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{29ACC7BB-E13D-4E0B-B061-D10D40E3677C}"/>
   <bookViews>
-    <workbookView xWindow="1140" yWindow="880" windowWidth="34860" windowHeight="22500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="5175" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -285,10 +285,11 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="3">
+  <numFmts count="4">
     <numFmt numFmtId="164" formatCode="#,##0.000"/>
     <numFmt numFmtId="165" formatCode="#,##0%"/>
     <numFmt numFmtId="166" formatCode="#,##0.00%"/>
+    <numFmt numFmtId="169" formatCode="0.0000"/>
   </numFmts>
   <fonts count="6" x14ac:knownFonts="1">
     <font>
@@ -391,7 +392,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="1" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -448,6 +449,9 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="2" fontId="5" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="169" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -757,47 +761,47 @@
   </sheetPr>
   <dimension ref="A1:AI47"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="I1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C1" sqref="C1"/>
+      <selection pane="bottomLeft" activeCell="T9" sqref="T9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.5" style="11" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="46.5" style="12" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.42578125" style="11" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="46.42578125" style="12" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="13" style="13" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="6.83203125" style="14" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="6.83203125" style="13" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.33203125" style="14" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="8.33203125" style="13" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="8.33203125" style="14" bestFit="1" customWidth="1"/>
-    <col min="10" max="11" width="8.33203125" style="12" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="6.85546875" style="14" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="6.85546875" style="13" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.28515625" style="14" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.28515625" style="13" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="8.28515625" style="14" bestFit="1" customWidth="1"/>
+    <col min="10" max="11" width="8.28515625" style="12" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="18" style="12" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="17.5" style="13" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="18.33203125" style="13" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="21.5" style="13" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="18.33203125" style="12" bestFit="1" customWidth="1"/>
-    <col min="17" max="19" width="18.33203125" style="13" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="26.83203125" style="12" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="17.1640625" style="12" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="15.5" style="13" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="14.5" style="12" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="14.1640625" style="12" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="14.1640625" style="13" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="14.1640625" style="12" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="13.5" style="15" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="17.42578125" style="13" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="18.28515625" style="13" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="21.42578125" style="13" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="18.28515625" style="12" bestFit="1" customWidth="1"/>
+    <col min="17" max="19" width="18.28515625" style="13" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="26.85546875" style="12" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="17.140625" style="12" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="15.42578125" style="13" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="14.42578125" style="12" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="14.140625" style="12" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="14.140625" style="13" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="14.140625" style="12" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="13.42578125" style="15" bestFit="1" customWidth="1"/>
     <col min="28" max="28" width="11" style="16" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="13.5" style="16" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="20.83203125" style="16" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="12.33203125" style="16" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="13.42578125" style="16" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="20.85546875" style="16" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="12.28515625" style="16" bestFit="1" customWidth="1"/>
     <col min="32" max="32" width="19" style="16" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="21.83203125" style="16" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="23.33203125" style="16" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="18.33203125" style="16" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="21.85546875" style="16" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="23.28515625" style="16" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="18.28515625" style="16" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:35" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:35" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -904,7 +908,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="2" spans="1:35" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:35" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>1111</v>
       </c>
@@ -974,7 +978,7 @@
         <f t="shared" ref="U2:U47" si="5">P2*T2</f>
         <v>367.51211252666258</v>
       </c>
-      <c r="V2" s="17">
+      <c r="V2" s="20">
         <v>0.7</v>
       </c>
       <c r="W2" s="17">
@@ -1020,7 +1024,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="3" spans="1:35" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:35" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>1121</v>
       </c>
@@ -1091,7 +1095,7 @@
         <f t="shared" si="5"/>
         <v>341.35244754201466</v>
       </c>
-      <c r="V3" s="17">
+      <c r="V3" s="20">
         <v>0.5</v>
       </c>
       <c r="W3" s="17">
@@ -1137,7 +1141,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:35" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:35" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>1122</v>
       </c>
@@ -1208,7 +1212,7 @@
         <f t="shared" si="5"/>
         <v>350.03285570940272</v>
       </c>
-      <c r="V4" s="17">
+      <c r="V4" s="20">
         <v>0.3</v>
       </c>
       <c r="W4" s="17">
@@ -1254,7 +1258,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:35" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:35" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>1123</v>
       </c>
@@ -1325,7 +1329,7 @@
         <f t="shared" si="5"/>
         <v>367.99570655700381</v>
       </c>
-      <c r="V5" s="17">
+      <c r="V5" s="20">
         <v>0.09</v>
       </c>
       <c r="W5" s="17">
@@ -1371,7 +1375,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:35" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:35" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>1130</v>
       </c>
@@ -1442,7 +1446,7 @@
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="V6" s="17">
+      <c r="V6" s="20">
         <v>0</v>
       </c>
       <c r="W6" s="17">
@@ -1488,7 +1492,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:35" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:35" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>1210</v>
       </c>
@@ -1559,7 +1563,7 @@
         <f t="shared" si="5"/>
         <v>500.29431259252556</v>
       </c>
-      <c r="V7" s="17">
+      <c r="V7" s="20">
         <v>0.45</v>
       </c>
       <c r="W7" s="17">
@@ -1605,7 +1609,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:35" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:35" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>1221</v>
       </c>
@@ -1676,7 +1680,7 @@
         <f t="shared" si="5"/>
         <v>485.00835417160897</v>
       </c>
-      <c r="V8" s="17">
+      <c r="V8" s="20">
         <v>0.05</v>
       </c>
       <c r="W8" s="17">
@@ -1722,7 +1726,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="9" spans="1:35" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:35" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>1222</v>
       </c>
@@ -1793,7 +1797,7 @@
         <f t="shared" si="5"/>
         <v>485.00835417160897</v>
       </c>
-      <c r="V9" s="17">
+      <c r="V9" s="20">
         <v>0.7</v>
       </c>
       <c r="W9" s="17">
@@ -1839,7 +1843,7 @@
         <v>0.6</v>
       </c>
     </row>
-    <row r="10" spans="1:35" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:35" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>1230</v>
       </c>
@@ -1910,7 +1914,7 @@
         <f t="shared" si="5"/>
         <v>485.00835417160897</v>
       </c>
-      <c r="V10" s="17">
+      <c r="V10" s="20">
         <v>0.3</v>
       </c>
       <c r="W10" s="17">
@@ -1956,7 +1960,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="11" spans="1:35" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:35" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>1241</v>
       </c>
@@ -2027,7 +2031,7 @@
         <f t="shared" si="5"/>
         <v>485.00835417160897</v>
       </c>
-      <c r="V11" s="17">
+      <c r="V11" s="20">
         <v>0.7</v>
       </c>
       <c r="W11" s="17">
@@ -2073,7 +2077,7 @@
         <v>0.6</v>
       </c>
     </row>
-    <row r="12" spans="1:35" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:35" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>1242</v>
       </c>
@@ -2144,7 +2148,7 @@
         <f t="shared" si="5"/>
         <v>485.00835417160897</v>
       </c>
-      <c r="V12" s="17">
+      <c r="V12" s="20">
         <v>0.7</v>
       </c>
       <c r="W12" s="17">
@@ -2190,7 +2194,7 @@
         <v>0.6</v>
       </c>
     </row>
-    <row r="13" spans="1:35" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:35" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>1310</v>
       </c>
@@ -2261,7 +2265,7 @@
         <f t="shared" si="5"/>
         <v>485.00835417160897</v>
       </c>
-      <c r="V13" s="17">
+      <c r="V13" s="20">
         <v>0.01</v>
       </c>
       <c r="W13" s="17">
@@ -2307,7 +2311,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:35" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:35" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>1320</v>
       </c>
@@ -2378,7 +2382,7 @@
         <f t="shared" si="5"/>
         <v>485.00835417160897</v>
       </c>
-      <c r="V14" s="17">
+      <c r="V14" s="20">
         <v>0.01</v>
       </c>
       <c r="W14" s="17">
@@ -2424,7 +2428,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:35" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:35" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>1330</v>
       </c>
@@ -2495,7 +2499,7 @@
         <f t="shared" si="5"/>
         <v>393.75526734897045</v>
       </c>
-      <c r="V15" s="17">
+      <c r="V15" s="20">
         <v>0.4</v>
       </c>
       <c r="W15" s="17">
@@ -2541,7 +2545,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:35" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:35" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>1410</v>
       </c>
@@ -2612,7 +2616,7 @@
         <f t="shared" si="5"/>
         <v>236.1336409725966</v>
       </c>
-      <c r="V16" s="17">
+      <c r="V16" s="20">
         <v>0.1</v>
       </c>
       <c r="W16" s="17">
@@ -2658,7 +2662,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:35" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:35" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>1421</v>
       </c>
@@ -2729,7 +2733,7 @@
         <f t="shared" si="5"/>
         <v>236.1336409725966</v>
       </c>
-      <c r="V17" s="17">
+      <c r="V17" s="20">
         <v>0.1</v>
       </c>
       <c r="W17" s="17">
@@ -2775,7 +2779,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:35" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:35" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>1422</v>
       </c>
@@ -2846,7 +2850,7 @@
         <f t="shared" si="5"/>
         <v>236.1336409725966</v>
       </c>
-      <c r="V18" s="17">
+      <c r="V18" s="20">
         <v>0.3</v>
       </c>
       <c r="W18" s="17">
@@ -2892,7 +2896,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:35" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:35" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>2110</v>
       </c>
@@ -2963,16 +2967,16 @@
         <f t="shared" si="5"/>
         <v>236.1336409725966</v>
       </c>
-      <c r="V19" s="17">
-        <v>7.0000000000000007E-2</v>
+      <c r="V19" s="20">
+        <v>1.5E-3</v>
       </c>
       <c r="W19" s="17">
         <f t="shared" si="6"/>
-        <v>33.058709736163529</v>
+        <v>0.70840092291778978</v>
       </c>
       <c r="X19" s="17">
         <f t="shared" si="7"/>
-        <v>16.529354868081764</v>
+        <v>0.35420046145889489</v>
       </c>
       <c r="Y19" s="17">
         <f t="shared" ref="Y19:Y29" si="10">0.1015744</f>
@@ -2980,7 +2984,7 @@
       </c>
       <c r="Z19" s="17">
         <f t="shared" si="8"/>
-        <v>49.689639004245286</v>
+        <v>1.1641757843766847</v>
       </c>
       <c r="AA19" s="18">
         <v>1</v>
@@ -3010,7 +3014,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:35" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:35" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <v>2120</v>
       </c>
@@ -3081,16 +3085,16 @@
         <f t="shared" si="5"/>
         <v>236.1336409725966</v>
       </c>
-      <c r="V20" s="17">
-        <v>7.0000000000000007E-2</v>
+      <c r="V20" s="20">
+        <v>1.5E-3</v>
       </c>
       <c r="W20" s="17">
         <f t="shared" si="6"/>
-        <v>33.058709736163529</v>
+        <v>0.70840092291778978</v>
       </c>
       <c r="X20" s="17">
         <f t="shared" si="7"/>
-        <v>16.529354868081764</v>
+        <v>0.35420046145889489</v>
       </c>
       <c r="Y20" s="17">
         <f t="shared" si="10"/>
@@ -3098,7 +3102,7 @@
       </c>
       <c r="Z20" s="17">
         <f t="shared" si="8"/>
-        <v>49.689639004245286</v>
+        <v>1.1641757843766847</v>
       </c>
       <c r="AA20" s="18">
         <v>1</v>
@@ -3128,7 +3132,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:35" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:35" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <v>2130</v>
       </c>
@@ -3199,16 +3203,16 @@
         <f t="shared" si="5"/>
         <v>236.1336409725966</v>
       </c>
-      <c r="V21" s="17">
-        <v>7.0000000000000007E-2</v>
+      <c r="V21" s="20">
+        <v>1.5E-3</v>
       </c>
       <c r="W21" s="17">
         <f t="shared" si="6"/>
-        <v>33.058709736163529</v>
+        <v>0.70840092291778978</v>
       </c>
       <c r="X21" s="17">
         <f t="shared" si="7"/>
-        <v>16.529354868081764</v>
+        <v>0.35420046145889489</v>
       </c>
       <c r="Y21" s="17">
         <f t="shared" si="10"/>
@@ -3216,7 +3220,7 @@
       </c>
       <c r="Z21" s="17">
         <f t="shared" si="8"/>
-        <v>49.689639004245286</v>
+        <v>1.1641757843766847</v>
       </c>
       <c r="AA21" s="18">
         <v>1</v>
@@ -3246,7 +3250,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:35" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:35" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <v>2210</v>
       </c>
@@ -3317,16 +3321,16 @@
         <f t="shared" si="5"/>
         <v>236.1336409725966</v>
       </c>
-      <c r="V22" s="17">
-        <v>7.0000000000000007E-2</v>
+      <c r="V22" s="20">
+        <v>1.5E-3</v>
       </c>
       <c r="W22" s="17">
         <f t="shared" si="6"/>
-        <v>33.058709736163529</v>
+        <v>0.70840092291778978</v>
       </c>
       <c r="X22" s="17">
         <f t="shared" si="7"/>
-        <v>16.529354868081764</v>
+        <v>0.35420046145889489</v>
       </c>
       <c r="Y22" s="17">
         <f t="shared" si="10"/>
@@ -3334,7 +3338,7 @@
       </c>
       <c r="Z22" s="17">
         <f t="shared" si="8"/>
-        <v>49.689639004245286</v>
+        <v>1.1641757843766847</v>
       </c>
       <c r="AA22" s="18">
         <v>1</v>
@@ -3364,7 +3368,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:35" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:35" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
         <v>2220</v>
       </c>
@@ -3435,16 +3439,16 @@
         <f t="shared" si="5"/>
         <v>236.1336409725966</v>
       </c>
-      <c r="V23" s="17">
-        <v>7.0000000000000007E-2</v>
+      <c r="V23" s="20">
+        <v>1.5E-3</v>
       </c>
       <c r="W23" s="17">
         <f t="shared" si="6"/>
-        <v>33.058709736163529</v>
+        <v>0.70840092291778978</v>
       </c>
       <c r="X23" s="17">
         <f t="shared" si="7"/>
-        <v>16.529354868081764</v>
+        <v>0.35420046145889489</v>
       </c>
       <c r="Y23" s="17">
         <f t="shared" si="10"/>
@@ -3452,7 +3456,7 @@
       </c>
       <c r="Z23" s="17">
         <f t="shared" si="8"/>
-        <v>49.689639004245286</v>
+        <v>1.1641757843766847</v>
       </c>
       <c r="AA23" s="18">
         <v>1</v>
@@ -3482,7 +3486,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:35" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:35" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
         <v>2230</v>
       </c>
@@ -3553,16 +3557,16 @@
         <f t="shared" si="5"/>
         <v>236.1336409725966</v>
       </c>
-      <c r="V24" s="17">
-        <v>7.0000000000000007E-2</v>
+      <c r="V24" s="20">
+        <v>1.5E-3</v>
       </c>
       <c r="W24" s="17">
         <f t="shared" si="6"/>
-        <v>33.058709736163529</v>
+        <v>0.70840092291778978</v>
       </c>
       <c r="X24" s="17">
         <f t="shared" si="7"/>
-        <v>16.529354868081764</v>
+        <v>0.35420046145889489</v>
       </c>
       <c r="Y24" s="17">
         <f t="shared" si="10"/>
@@ -3570,7 +3574,7 @@
       </c>
       <c r="Z24" s="17">
         <f t="shared" si="8"/>
-        <v>49.689639004245286</v>
+        <v>1.1641757843766847</v>
       </c>
       <c r="AA24" s="18">
         <v>1</v>
@@ -3600,7 +3604,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:35" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:35" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
         <v>2310</v>
       </c>
@@ -3671,16 +3675,16 @@
         <f t="shared" si="5"/>
         <v>236.1336409725966</v>
       </c>
-      <c r="V25" s="17">
-        <v>7.0000000000000007E-2</v>
+      <c r="V25" s="20">
+        <v>1.5E-3</v>
       </c>
       <c r="W25" s="17">
         <f t="shared" si="6"/>
-        <v>33.058709736163529</v>
+        <v>0.70840092291778978</v>
       </c>
       <c r="X25" s="17">
         <f t="shared" si="7"/>
-        <v>16.529354868081764</v>
+        <v>0.35420046145889489</v>
       </c>
       <c r="Y25" s="17">
         <f t="shared" si="10"/>
@@ -3688,7 +3692,7 @@
       </c>
       <c r="Z25" s="17">
         <f t="shared" si="8"/>
-        <v>49.689639004245286</v>
+        <v>1.1641757843766847</v>
       </c>
       <c r="AA25" s="18">
         <v>1</v>
@@ -3718,7 +3722,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:35" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:35" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
         <v>2410</v>
       </c>
@@ -3789,16 +3793,16 @@
         <f t="shared" si="5"/>
         <v>236.1336409725966</v>
       </c>
-      <c r="V26" s="17">
-        <v>7.0000000000000007E-2</v>
+      <c r="V26" s="20">
+        <v>1.5E-3</v>
       </c>
       <c r="W26" s="17">
         <f t="shared" si="6"/>
-        <v>33.058709736163529</v>
+        <v>0.70840092291778978</v>
       </c>
       <c r="X26" s="17">
         <f t="shared" si="7"/>
-        <v>16.529354868081764</v>
+        <v>0.35420046145889489</v>
       </c>
       <c r="Y26" s="17">
         <f t="shared" si="10"/>
@@ -3806,7 +3810,7 @@
       </c>
       <c r="Z26" s="17">
         <f t="shared" si="8"/>
-        <v>49.689639004245286</v>
+        <v>1.1641757843766847</v>
       </c>
       <c r="AA26" s="18">
         <v>1</v>
@@ -3836,7 +3840,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:35" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:35" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
         <v>2420</v>
       </c>
@@ -3907,16 +3911,16 @@
         <f t="shared" si="5"/>
         <v>236.1336409725966</v>
       </c>
-      <c r="V27" s="17">
-        <v>7.0000000000000007E-2</v>
+      <c r="V27" s="20">
+        <v>1.5E-3</v>
       </c>
       <c r="W27" s="17">
         <f t="shared" si="6"/>
-        <v>33.058709736163529</v>
+        <v>0.70840092291778978</v>
       </c>
       <c r="X27" s="17">
         <f t="shared" si="7"/>
-        <v>16.529354868081764</v>
+        <v>0.35420046145889489</v>
       </c>
       <c r="Y27" s="17">
         <f t="shared" si="10"/>
@@ -3924,7 +3928,7 @@
       </c>
       <c r="Z27" s="17">
         <f t="shared" si="8"/>
-        <v>49.689639004245286</v>
+        <v>1.1641757843766847</v>
       </c>
       <c r="AA27" s="18">
         <v>1</v>
@@ -3954,7 +3958,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:35" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:35" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
         <v>2430</v>
       </c>
@@ -4025,16 +4029,16 @@
         <f t="shared" si="5"/>
         <v>236.1336409725966</v>
       </c>
-      <c r="V28" s="17">
-        <v>7.0000000000000007E-2</v>
+      <c r="V28" s="20">
+        <v>1.5E-3</v>
       </c>
       <c r="W28" s="17">
         <f t="shared" si="6"/>
-        <v>33.058709736163529</v>
+        <v>0.70840092291778978</v>
       </c>
       <c r="X28" s="17">
         <f t="shared" si="7"/>
-        <v>16.529354868081764</v>
+        <v>0.35420046145889489</v>
       </c>
       <c r="Y28" s="17">
         <f t="shared" si="10"/>
@@ -4042,7 +4046,7 @@
       </c>
       <c r="Z28" s="17">
         <f t="shared" si="8"/>
-        <v>49.689639004245286</v>
+        <v>1.1641757843766847</v>
       </c>
       <c r="AA28" s="18">
         <v>1</v>
@@ -4072,7 +4076,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:35" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:35" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
         <v>2440</v>
       </c>
@@ -4143,16 +4147,16 @@
         <f t="shared" si="5"/>
         <v>236.1336409725966</v>
       </c>
-      <c r="V29" s="17">
-        <v>7.0000000000000007E-2</v>
+      <c r="V29" s="20">
+        <v>1.5E-3</v>
       </c>
       <c r="W29" s="17">
         <f t="shared" si="6"/>
-        <v>33.058709736163529</v>
+        <v>0.70840092291778978</v>
       </c>
       <c r="X29" s="17">
         <f t="shared" si="7"/>
-        <v>16.529354868081764</v>
+        <v>0.35420046145889489</v>
       </c>
       <c r="Y29" s="17">
         <f t="shared" si="10"/>
@@ -4160,7 +4164,7 @@
       </c>
       <c r="Z29" s="17">
         <f t="shared" si="8"/>
-        <v>49.689639004245286</v>
+        <v>1.1641757843766847</v>
       </c>
       <c r="AA29" s="18">
         <v>1</v>
@@ -4190,7 +4194,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:35" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:35" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
         <v>3110</v>
       </c>
@@ -4261,7 +4265,7 @@
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="V30" s="17">
+      <c r="V30" s="20">
         <v>0</v>
       </c>
       <c r="W30" s="17">
@@ -4307,7 +4311,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:35" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:35" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
         <v>3120</v>
       </c>
@@ -4378,7 +4382,7 @@
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="V31" s="17">
+      <c r="V31" s="20">
         <v>0</v>
       </c>
       <c r="W31" s="17">
@@ -4424,7 +4428,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:35" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:35" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="1">
         <v>3130</v>
       </c>
@@ -4495,7 +4499,7 @@
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="V32" s="17">
+      <c r="V32" s="20">
         <v>0</v>
       </c>
       <c r="W32" s="17">
@@ -4541,7 +4545,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:35" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:35" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="1">
         <v>3210</v>
       </c>
@@ -4612,23 +4616,23 @@
         <f t="shared" si="5"/>
         <v>236.1336409725966</v>
       </c>
-      <c r="V33" s="17">
-        <v>7.0000000000000007E-2</v>
+      <c r="V33" s="20">
+        <v>1.5E-3</v>
       </c>
       <c r="W33" s="17">
         <f t="shared" si="6"/>
-        <v>33.058709736163529</v>
+        <v>0.70840092291778978</v>
       </c>
       <c r="X33" s="17">
         <f t="shared" si="7"/>
-        <v>16.529354868081764</v>
+        <v>0.35420046145889489</v>
       </c>
       <c r="Y33" s="17">
         <v>0</v>
       </c>
       <c r="Z33" s="17">
         <f t="shared" si="8"/>
-        <v>49.58806460424529</v>
+        <v>1.0626013843766846</v>
       </c>
       <c r="AA33" s="18">
         <v>1</v>
@@ -4658,7 +4662,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:35" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:35" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="1">
         <v>3220</v>
       </c>
@@ -4729,23 +4733,23 @@
         <f t="shared" si="5"/>
         <v>236.1336409725966</v>
       </c>
-      <c r="V34" s="17">
-        <v>7.0000000000000007E-2</v>
+      <c r="V34" s="20">
+        <v>1.5E-3</v>
       </c>
       <c r="W34" s="17">
         <f t="shared" si="6"/>
-        <v>33.058709736163529</v>
+        <v>0.70840092291778978</v>
       </c>
       <c r="X34" s="17">
         <f t="shared" si="7"/>
-        <v>16.529354868081764</v>
+        <v>0.35420046145889489</v>
       </c>
       <c r="Y34" s="17">
         <v>0</v>
       </c>
       <c r="Z34" s="17">
         <f t="shared" si="8"/>
-        <v>49.58806460424529</v>
+        <v>1.0626013843766846</v>
       </c>
       <c r="AA34" s="18">
         <v>1</v>
@@ -4775,7 +4779,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:35" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:35" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="1">
         <v>3230</v>
       </c>
@@ -4846,23 +4850,23 @@
         <f t="shared" si="5"/>
         <v>236.1336409725966</v>
       </c>
-      <c r="V35" s="17">
-        <v>7.0000000000000007E-2</v>
+      <c r="V35" s="20">
+        <v>1.5E-3</v>
       </c>
       <c r="W35" s="17">
         <f t="shared" si="6"/>
-        <v>33.058709736163529</v>
+        <v>0.70840092291778978</v>
       </c>
       <c r="X35" s="17">
         <f t="shared" si="7"/>
-        <v>16.529354868081764</v>
+        <v>0.35420046145889489</v>
       </c>
       <c r="Y35" s="17">
         <v>0</v>
       </c>
       <c r="Z35" s="17">
         <f t="shared" si="8"/>
-        <v>49.58806460424529</v>
+        <v>1.0626013843766846</v>
       </c>
       <c r="AA35" s="18">
         <v>1</v>
@@ -4892,7 +4896,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:35" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:35" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="1">
         <v>3240</v>
       </c>
@@ -4963,23 +4967,23 @@
         <f t="shared" si="5"/>
         <v>236.1336409725966</v>
       </c>
-      <c r="V36" s="17">
-        <v>7.0000000000000007E-2</v>
+      <c r="V36" s="20">
+        <v>1.5E-3</v>
       </c>
       <c r="W36" s="17">
         <f t="shared" si="6"/>
-        <v>33.058709736163529</v>
+        <v>0.70840092291778978</v>
       </c>
       <c r="X36" s="17">
         <f t="shared" si="7"/>
-        <v>16.529354868081764</v>
+        <v>0.35420046145889489</v>
       </c>
       <c r="Y36" s="17">
         <v>0</v>
       </c>
       <c r="Z36" s="17">
         <f t="shared" si="8"/>
-        <v>49.58806460424529</v>
+        <v>1.0626013843766846</v>
       </c>
       <c r="AA36" s="18">
         <v>1</v>
@@ -5009,7 +5013,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:35" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:35" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="1">
         <v>3310</v>
       </c>
@@ -5080,23 +5084,23 @@
         <f t="shared" si="5"/>
         <v>236.1336409725966</v>
       </c>
-      <c r="V37" s="17">
-        <v>7.0000000000000007E-2</v>
+      <c r="V37" s="20">
+        <v>1.5E-3</v>
       </c>
       <c r="W37" s="17">
         <f t="shared" si="6"/>
-        <v>33.058709736163529</v>
+        <v>0.70840092291778978</v>
       </c>
       <c r="X37" s="17">
         <f t="shared" si="7"/>
-        <v>16.529354868081764</v>
+        <v>0.35420046145889489</v>
       </c>
       <c r="Y37" s="17">
         <v>0</v>
       </c>
       <c r="Z37" s="17">
         <f t="shared" si="8"/>
-        <v>49.58806460424529</v>
+        <v>1.0626013843766846</v>
       </c>
       <c r="AA37" s="18">
         <v>1</v>
@@ -5126,7 +5130,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:35" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:35" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="1">
         <v>3320</v>
       </c>
@@ -5197,23 +5201,23 @@
         <f t="shared" si="5"/>
         <v>236.1336409725966</v>
       </c>
-      <c r="V38" s="17">
-        <v>7.0000000000000007E-2</v>
+      <c r="V38" s="20">
+        <v>1.5E-3</v>
       </c>
       <c r="W38" s="17">
         <f t="shared" si="6"/>
-        <v>33.058709736163529</v>
+        <v>0.70840092291778978</v>
       </c>
       <c r="X38" s="17">
         <f t="shared" si="7"/>
-        <v>16.529354868081764</v>
+        <v>0.35420046145889489</v>
       </c>
       <c r="Y38" s="17">
         <v>0</v>
       </c>
       <c r="Z38" s="17">
         <f t="shared" si="8"/>
-        <v>49.58806460424529</v>
+        <v>1.0626013843766846</v>
       </c>
       <c r="AA38" s="18">
         <v>1</v>
@@ -5243,7 +5247,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:35" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:35" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="1">
         <v>3330</v>
       </c>
@@ -5314,23 +5318,23 @@
         <f t="shared" si="5"/>
         <v>236.1336409725966</v>
       </c>
-      <c r="V39" s="17">
-        <v>7.0000000000000007E-2</v>
+      <c r="V39" s="20">
+        <v>1.5E-3</v>
       </c>
       <c r="W39" s="17">
         <f t="shared" si="6"/>
-        <v>33.058709736163529</v>
+        <v>0.70840092291778978</v>
       </c>
       <c r="X39" s="17">
         <f t="shared" si="7"/>
-        <v>16.529354868081764</v>
+        <v>0.35420046145889489</v>
       </c>
       <c r="Y39" s="17">
         <v>0</v>
       </c>
       <c r="Z39" s="17">
         <f t="shared" si="8"/>
-        <v>49.58806460424529</v>
+        <v>1.0626013843766846</v>
       </c>
       <c r="AA39" s="18">
         <v>1</v>
@@ -5360,7 +5364,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:35" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:35" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="1">
         <v>3340</v>
       </c>
@@ -5431,23 +5435,23 @@
         <f t="shared" si="5"/>
         <v>236.1336409725966</v>
       </c>
-      <c r="V40" s="17">
-        <v>7.0000000000000007E-2</v>
+      <c r="V40" s="20">
+        <v>1.5E-3</v>
       </c>
       <c r="W40" s="17">
         <f t="shared" si="6"/>
-        <v>33.058709736163529</v>
+        <v>0.70840092291778978</v>
       </c>
       <c r="X40" s="17">
         <f t="shared" si="7"/>
-        <v>16.529354868081764</v>
+        <v>0.35420046145889489</v>
       </c>
       <c r="Y40" s="17">
         <v>0</v>
       </c>
       <c r="Z40" s="17">
         <f t="shared" si="8"/>
-        <v>49.58806460424529</v>
+        <v>1.0626013843766846</v>
       </c>
       <c r="AA40" s="18">
         <v>1</v>
@@ -5477,7 +5481,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:35" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:35" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="1">
         <v>3350</v>
       </c>
@@ -5548,23 +5552,23 @@
         <f t="shared" si="5"/>
         <v>236.1336409725966</v>
       </c>
-      <c r="V41" s="17">
-        <v>7.0000000000000007E-2</v>
+      <c r="V41" s="20">
+        <v>1.5E-3</v>
       </c>
       <c r="W41" s="17">
         <f t="shared" si="6"/>
-        <v>33.058709736163529</v>
+        <v>0.70840092291778978</v>
       </c>
       <c r="X41" s="17">
         <f t="shared" si="7"/>
-        <v>16.529354868081764</v>
+        <v>0.35420046145889489</v>
       </c>
       <c r="Y41" s="17">
         <v>0</v>
       </c>
       <c r="Z41" s="17">
         <f t="shared" si="8"/>
-        <v>49.58806460424529</v>
+        <v>1.0626013843766846</v>
       </c>
       <c r="AA41" s="18">
         <v>1</v>
@@ -5594,7 +5598,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:35" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:35" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="1">
         <v>4000</v>
       </c>
@@ -5665,23 +5669,23 @@
         <f t="shared" si="5"/>
         <v>236.1336409725966</v>
       </c>
-      <c r="V42" s="17">
-        <v>7.0000000000000007E-2</v>
+      <c r="V42" s="20">
+        <v>1.5E-3</v>
       </c>
       <c r="W42" s="17">
         <f t="shared" si="6"/>
-        <v>33.058709736163529</v>
+        <v>0.70840092291778978</v>
       </c>
       <c r="X42" s="17">
         <f t="shared" si="7"/>
-        <v>16.529354868081764</v>
+        <v>0.35420046145889489</v>
       </c>
       <c r="Y42" s="17">
         <v>0</v>
       </c>
       <c r="Z42" s="17">
         <f t="shared" si="8"/>
-        <v>49.58806460424529</v>
+        <v>1.0626013843766846</v>
       </c>
       <c r="AA42" s="18">
         <v>1</v>
@@ -5711,7 +5715,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:35" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:35" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="1">
         <v>5110</v>
       </c>
@@ -5782,7 +5786,7 @@
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="V43" s="17">
+      <c r="V43" s="20">
         <v>0</v>
       </c>
       <c r="W43" s="17">
@@ -5828,7 +5832,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:35" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:35" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="1">
         <v>5120</v>
       </c>
@@ -5899,7 +5903,7 @@
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="V44" s="17">
+      <c r="V44" s="20">
         <v>0</v>
       </c>
       <c r="W44" s="17">
@@ -5945,7 +5949,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:35" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:35" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="1">
         <v>5210</v>
       </c>
@@ -6016,7 +6020,7 @@
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="V45" s="17">
+      <c r="V45" s="20">
         <v>0</v>
       </c>
       <c r="W45" s="17">
@@ -6062,7 +6066,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:35" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:35" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="1">
         <v>5220</v>
       </c>
@@ -6133,7 +6137,7 @@
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="V46" s="17">
+      <c r="V46" s="20">
         <v>0</v>
       </c>
       <c r="W46" s="17">
@@ -6179,7 +6183,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:35" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:35" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="1">
         <v>5230</v>
       </c>
@@ -6250,7 +6254,7 @@
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="V47" s="17">
+      <c r="V47" s="20">
         <v>0</v>
       </c>
       <c r="W47" s="17">

</xml_diff>